<commit_message>
Project Example 1 - Bank Rating is saved. Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Example 1 - Bank Rating/Bank Rating.xlsx
+++ b/DESIGN/rules/Example 1 - Bank Rating/Bank Rating.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="694">
   <si>
     <t xml:space="preserve">www.commerzbank.com</t>
   </si>
@@ -4374,6 +4374,9 @@
   </si>
   <si>
     <t xml:space="preserve">SPD</t>
+  </si>
+  <si>
+    <t>Bank Rating1</t>
   </si>
 </sst>
 </file>
@@ -5622,47 +5625,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+  <cellStyleXfs count="4">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true" xfId="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true" xfId="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true" xfId="2">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false" xfId="3">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -5675,7 +5651,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5683,7 +5659,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5723,7 +5699,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5739,7 +5715,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5791,7 +5767,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6403,7 +6379,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="102" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="102" xfId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6463,7 +6439,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="29" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="29" xfId="2" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6495,23 +6471,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="67" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="67" xfId="2" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Normal 7" xfId="21"/>
-    <cellStyle name="Normal_EPLI rater" xfId="22"/>
-    <cellStyle name="Обычный 2" xfId="23"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
-    <cellStyle name="Excel Built-in Heading 1" xfId="24"/>
+    <cellStyle name="*unknown*" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal_EPLI rater" xfId="2"/>
+    <cellStyle name="Excel Built-in Heading 1" xfId="3"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -6660,16 +6629,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="76.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="5.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="9.11"/>
+    <col min="1" max="2" customWidth="false" hidden="false" style="1" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="8.56" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="16.56" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="25.66" collapsed="false" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="42.34" collapsed="false" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="76.67" collapsed="false" outlineLevel="0"/>
+    <col min="8" max="9" customWidth="true" hidden="false" style="1" width="5.88" collapsed="false" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="24.99" collapsed="false" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="1" width="19.11" collapsed="false" outlineLevel="0"/>
+    <col min="12" max="1024" customWidth="false" hidden="false" style="1" width="9.11" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7688,9 +7657,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.66"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="27.11" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="27.44" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="31.66" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7882,9 +7851,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="24.99" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="31.66" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="36.0" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7931,7 +7900,7 @@
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="11" t="s">
-        <v>388</v>
+        <v>693</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>187</v>
@@ -8024,8 +7993,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.66"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="22.66" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="25.66" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8123,18 +8092,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="12.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.89"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="4.33" collapsed="false" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="3.89" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="9.88" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="24.01" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="44.45" collapsed="false" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="30.89" collapsed="false" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="0" width="11.56" collapsed="false" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="11.99" collapsed="false" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="11.56" collapsed="false" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="0" width="11.1" collapsed="false" outlineLevel="0"/>
+    <col min="11" max="12" customWidth="true" hidden="false" style="0" width="12.11" collapsed="false" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="0" width="12.89" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8650,9 +8619,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.34"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="20.66" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="30.56" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="19.34" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8735,11 +8704,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="95" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="95" width="14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="95" width="9.11"/>
+    <col min="1" max="2" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="95" width="18.22" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="95" width="13.56" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="95" width="14.0" collapsed="false" outlineLevel="0"/>
+    <col min="6" max="1024" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8817,8 +8786,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="76.22"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="28.44" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="76.22" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8991,8 +8960,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.11"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="20.44" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="26.11" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9070,10 +9039,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="95" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="39.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="95" width="9.11"/>
+    <col min="1" max="2" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="95" width="17.67" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="95" width="39.11" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="1024" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9503,10 +9472,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="95" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="34.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="95" width="29.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="95" width="9.11"/>
+    <col min="1" max="3" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="95" width="34.44" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="95" width="29.99" collapsed="false" outlineLevel="0"/>
+    <col min="6" max="1024" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9910,9 +9879,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.11"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="21.33" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="38.01" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="22.11" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10182,27 +10151,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="95" width="3.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="95" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="19.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="20.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="95" width="28.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="95" width="24.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="95" width="51.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="95" width="30.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="95" width="32.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="95" width="48.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="95" width="29.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="95" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="95" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="95" width="12.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="95" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="95" width="25.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="95" width="24.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="95" width="38.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="95" width="23.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="95" width="19.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="21" style="95" width="9.11"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="95" width="3.56" collapsed="false" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="95" width="19.11" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="95" width="20.99" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="95" width="28.44" collapsed="false" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="95" width="24.99" collapsed="false" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="95" width="51.66" collapsed="false" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="95" width="30.11" collapsed="false" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="95" width="32.66" collapsed="false" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="95" width="48.56" collapsed="false" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="95" width="29.89" collapsed="false" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="95" width="9.66" collapsed="false" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="95" width="10.0" collapsed="false" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="95" width="12.45" collapsed="false" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="95" width="21.67" collapsed="false" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="95" width="25.89" collapsed="false" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="95" width="24.99" collapsed="false" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="95" width="38.66" collapsed="false" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="95" width="23.11" collapsed="false" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="95" width="19.44" collapsed="false" outlineLevel="0"/>
+    <col min="21" max="1024" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11424,10 +11393,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.88"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="43.56" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="34.32" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="9.88" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12145,10 +12114,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.56"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="14.11" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="23.11" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="27.11" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="24.56" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12239,9 +12208,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.33"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="29.99" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="31.66" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="26.33" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12526,9 +12495,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="14.88" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="23.11" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="22.0" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12639,8 +12608,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="31.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.11"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="0" width="31.33" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="22.11" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12979,9 +12948,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.67"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="18.88" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="22.33" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="21.67" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13132,12 +13101,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.33"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="44.89" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="40.44" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="35.33" collapsed="false" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="15.1" collapsed="false" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="26.33" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Project Example 1 - Bank Rating is saved. Author: user. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Example 1 - Bank Rating/Bank Rating.xlsx
+++ b/DESIGN/rules/Example 1 - Bank Rating/Bank Rating.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="706">
   <si>
     <t xml:space="preserve">www.commerzbank.com</t>
   </si>
@@ -4377,6 +4377,42 @@
   </si>
   <si>
     <t>Bank Rating1</t>
+  </si>
+  <si>
+    <t>SimpleRules RatingGroup BankRatingGroup1 (Double bankRating)</t>
+  </si>
+  <si>
+    <t>&lt;= 0.25</t>
+  </si>
+  <si>
+    <t>(0.25 .. 0.4]</t>
+  </si>
+  <si>
+    <t>(0.4 .. 0.7]</t>
+  </si>
+  <si>
+    <t>(0.7 .. 0.9]</t>
+  </si>
+  <si>
+    <t>&gt; 0.9</t>
+  </si>
+  <si>
+    <t>Bank Rating Group</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R1</t>
   </si>
 </sst>
 </file>
@@ -6621,7 +6657,7 @@
     <tabColor rgb="FF558ED5"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:J96"/>
+  <dimension ref="B1:J104"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
@@ -7542,8 +7578,62 @@
         <v>179</v>
       </c>
     </row>
+    <row r="98">
+      <c r="B98" s="7" t="s">
+        <v>694</v>
+      </c>
+      <c r="C98" s="7"/>
+    </row>
+    <row r="99">
+      <c r="B99" t="s" s="11">
+        <v>693</v>
+      </c>
+      <c r="C99" t="s" s="13">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="s" s="64">
+        <v>695</v>
+      </c>
+      <c r="C100" t="s" s="65">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="s" s="67">
+        <v>696</v>
+      </c>
+      <c r="C101" t="s" s="68">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="s" s="67">
+        <v>697</v>
+      </c>
+      <c r="C102" t="s" s="68">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="s" s="67">
+        <v>698</v>
+      </c>
+      <c r="C103" t="s" s="68">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="s" s="69">
+        <v>699</v>
+      </c>
+      <c r="C104" t="s" s="70">
+        <v>705</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="77">
+  <mergeCells count="78">
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="F10:G10"/>
@@ -7621,6 +7711,7 @@
     <mergeCell ref="D94:E94"/>
     <mergeCell ref="D95:E95"/>
     <mergeCell ref="D96:E96"/>
+    <mergeCell ref="B98:C98"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J1" r:id="rId1" display="www.commerzbank.com"/>

</xml_diff>

<commit_message>
Project Example 1 - Bank Rating is created. Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Example 1 - Bank Rating/Bank Rating.xlsx
+++ b/DESIGN/rules/Example 1 - Bank Rating/Bank Rating.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="693">
   <si>
     <t xml:space="preserve">www.commerzbank.com</t>
   </si>
@@ -4374,45 +4374,6 @@
   </si>
   <si>
     <t xml:space="preserve">SPD</t>
-  </si>
-  <si>
-    <t>Bank Rating1</t>
-  </si>
-  <si>
-    <t>SimpleRules RatingGroup BankRatingGroup1 (Double bankRating)</t>
-  </si>
-  <si>
-    <t>&lt;= 0.25</t>
-  </si>
-  <si>
-    <t>(0.25 .. 0.4]</t>
-  </si>
-  <si>
-    <t>(0.4 .. 0.7]</t>
-  </si>
-  <si>
-    <t>(0.7 .. 0.9]</t>
-  </si>
-  <si>
-    <t>&gt; 0.9</t>
-  </si>
-  <si>
-    <t>Bank Rating Group</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R1</t>
   </si>
 </sst>
 </file>
@@ -5661,20 +5622,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true" xfId="0">
+  <cellStyleXfs count="25">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true" xfId="2">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false" xfId="3">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -5687,7 +5675,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5695,7 +5683,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5735,7 +5723,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5751,7 +5739,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5803,7 +5791,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6415,7 +6403,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="102" xfId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="102" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6475,7 +6463,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="29" xfId="2" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="29" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6507,16 +6495,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="67" xfId="2" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="67" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="11">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="*unknown*" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal_EPLI rater" xfId="2"/>
-    <cellStyle name="Excel Built-in Heading 1" xfId="3"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal 7" xfId="21"/>
+    <cellStyle name="Normal_EPLI rater" xfId="22"/>
+    <cellStyle name="Обычный 2" xfId="23"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+    <cellStyle name="Excel Built-in Heading 1" xfId="24"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -6657,7 +6652,7 @@
     <tabColor rgb="FF558ED5"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:J104"/>
+  <dimension ref="B1:J96"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
@@ -6665,16 +6660,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" customWidth="false" hidden="false" style="1" width="9.11" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="8.56" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="16.56" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="25.66" collapsed="false" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="42.34" collapsed="false" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="76.67" collapsed="false" outlineLevel="0"/>
-    <col min="8" max="9" customWidth="true" hidden="false" style="1" width="5.88" collapsed="false" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="24.99" collapsed="false" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="1" width="19.11" collapsed="false" outlineLevel="0"/>
-    <col min="12" max="1024" customWidth="false" hidden="false" style="1" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="76.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="9.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7578,62 +7573,8 @@
         <v>179</v>
       </c>
     </row>
-    <row r="98">
-      <c r="B98" s="7" t="s">
-        <v>694</v>
-      </c>
-      <c r="C98" s="7"/>
-    </row>
-    <row r="99">
-      <c r="B99" t="s" s="11">
-        <v>693</v>
-      </c>
-      <c r="C99" t="s" s="13">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="B100" t="s" s="64">
-        <v>695</v>
-      </c>
-      <c r="C100" t="s" s="65">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="B101" t="s" s="67">
-        <v>696</v>
-      </c>
-      <c r="C101" t="s" s="68">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="B102" t="s" s="67">
-        <v>697</v>
-      </c>
-      <c r="C102" t="s" s="68">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="B103" t="s" s="67">
-        <v>698</v>
-      </c>
-      <c r="C103" t="s" s="68">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="B104" t="s" s="69">
-        <v>699</v>
-      </c>
-      <c r="C104" t="s" s="70">
-        <v>705</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="78">
+  <mergeCells count="77">
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="F10:G10"/>
@@ -7711,7 +7652,6 @@
     <mergeCell ref="D94:E94"/>
     <mergeCell ref="D95:E95"/>
     <mergeCell ref="D96:E96"/>
-    <mergeCell ref="B98:C98"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J1" r:id="rId1" display="www.commerzbank.com"/>
@@ -7748,9 +7688,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="27.11" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="27.44" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="31.66" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.66"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7942,9 +7882,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="24.99" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="31.66" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="36.0" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7991,7 +7931,7 @@
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="11" t="s">
-        <v>693</v>
+        <v>388</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>187</v>
@@ -8084,8 +8024,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="22.66" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="25.66" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.66"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8183,18 +8123,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="4.33" collapsed="false" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="3.89" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="9.88" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="24.01" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="44.45" collapsed="false" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="30.89" collapsed="false" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="0" width="11.56" collapsed="false" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="11.99" collapsed="false" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="11.56" collapsed="false" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="0" width="11.1" collapsed="false" outlineLevel="0"/>
-    <col min="11" max="12" customWidth="true" hidden="false" style="0" width="12.11" collapsed="false" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="0" width="12.89" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="12.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8710,9 +8650,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="20.66" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="30.56" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="19.34" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.34"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8795,11 +8735,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="95" width="18.22" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="95" width="13.56" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="95" width="14.0" collapsed="false" outlineLevel="0"/>
-    <col min="6" max="1024" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="95" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="95" width="14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="95" width="9.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8877,8 +8817,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="28.44" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="76.22" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="76.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9051,8 +8991,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="20.44" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="26.11" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.11"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9130,10 +9070,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="95" width="17.67" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="95" width="39.11" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="1024" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="95" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="39.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="95" width="9.11"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9563,10 +9503,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="95" width="34.44" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="95" width="29.99" collapsed="false" outlineLevel="0"/>
-    <col min="6" max="1024" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="95" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="34.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="95" width="29.99"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="95" width="9.11"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9970,9 +9910,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="21.33" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="38.01" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="22.11" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.11"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10242,27 +10182,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="95" width="3.56" collapsed="false" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="95" width="19.11" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="95" width="20.99" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="95" width="28.44" collapsed="false" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="95" width="24.99" collapsed="false" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="95" width="51.66" collapsed="false" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="95" width="30.11" collapsed="false" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="95" width="32.66" collapsed="false" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="95" width="48.56" collapsed="false" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="95" width="29.89" collapsed="false" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="95" width="9.66" collapsed="false" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="95" width="10.0" collapsed="false" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="95" width="12.45" collapsed="false" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="95" width="21.67" collapsed="false" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="95" width="25.89" collapsed="false" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="95" width="24.99" collapsed="false" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="95" width="38.66" collapsed="false" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="95" width="23.11" collapsed="false" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="95" width="19.44" collapsed="false" outlineLevel="0"/>
-    <col min="21" max="1024" customWidth="false" hidden="false" style="95" width="9.11" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="95" width="3.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="95" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="95" width="28.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="95" width="24.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="95" width="51.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="95" width="30.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="95" width="32.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="95" width="48.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="95" width="29.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="95" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="95" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="95" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="95" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="95" width="25.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="95" width="24.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="95" width="38.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="95" width="23.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="95" width="19.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="21" style="95" width="9.11"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11484,10 +11424,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.11" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="43.56" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="34.32" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="9.88" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12205,10 +12145,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="14.11" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="23.11" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="27.11" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="24.56" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.56"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12299,9 +12239,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="29.99" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="31.66" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="26.33" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.33"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12586,9 +12526,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="14.88" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="23.11" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="22.0" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12699,8 +12639,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="4" customWidth="true" hidden="false" style="0" width="31.33" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="22.11" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="31.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13039,9 +12979,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="18.88" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="22.33" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="21.67" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.67"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13192,12 +13132,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.11" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="44.89" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="40.44" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="35.33" collapsed="false" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="15.1" collapsed="false" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="26.33" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>